<commit_message>
QMM008 update template B
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_厚生年金保険料率一覧.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_厚生年金保険料率一覧.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$T$118</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1562,30 +1562,57 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="66" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="64" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="62" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="48" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1598,38 +1625,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="64" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="62" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2000,67 +2000,67 @@
       <c r="S1" s="21"/>
     </row>
     <row r="2" spans="1:19" s="7" customFormat="1" ht="15.75" thickTop="1">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="99" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="54"/>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114" t="s">
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="115"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="106"/>
       <c r="S2" s="55"/>
     </row>
     <row r="3" spans="1:19" s="7" customFormat="1" ht="15">
-      <c r="B3" s="108"/>
-      <c r="C3" s="95"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="100"/>
       <c r="D3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="99" t="s">
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="99"/>
-      <c r="J3" s="116"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="100" t="s">
+      <c r="L3" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="99" t="s">
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="116"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="110"/>
       <c r="R3" s="93"/>
       <c r="S3" s="55"/>
     </row>
     <row r="4" spans="1:19" s="7" customFormat="1" ht="60.75" thickBot="1">
       <c r="A4" s="74"/>
-      <c r="B4" s="109"/>
-      <c r="C4" s="96"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="19" t="s">
         <v>22</v>
       </c>
@@ -3280,7 +3280,7 @@
       <c r="M60" s="53"/>
       <c r="N60" s="53"/>
       <c r="O60" s="53"/>
-      <c r="P60" s="117" t="s">
+      <c r="P60" s="95" t="s">
         <v>25</v>
       </c>
       <c r="Q60" s="53"/>
@@ -3291,68 +3291,68 @@
     </row>
     <row r="61" spans="1:19" s="7" customFormat="1" ht="15.75" thickTop="1">
       <c r="A61" s="74"/>
-      <c r="B61" s="97" t="s">
+      <c r="B61" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="95" t="s">
+      <c r="C61" s="100" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="18"/>
-      <c r="E61" s="106" t="s">
+      <c r="E61" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="F61" s="104"/>
-      <c r="G61" s="104"/>
-      <c r="H61" s="104"/>
-      <c r="I61" s="104"/>
-      <c r="J61" s="104"/>
-      <c r="K61" s="105"/>
-      <c r="L61" s="103" t="s">
+      <c r="F61" s="113"/>
+      <c r="G61" s="113"/>
+      <c r="H61" s="113"/>
+      <c r="I61" s="113"/>
+      <c r="J61" s="113"/>
+      <c r="K61" s="114"/>
+      <c r="L61" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="M61" s="104"/>
-      <c r="N61" s="104"/>
-      <c r="O61" s="104"/>
-      <c r="P61" s="104"/>
-      <c r="Q61" s="104"/>
-      <c r="R61" s="105"/>
+      <c r="M61" s="113"/>
+      <c r="N61" s="113"/>
+      <c r="O61" s="113"/>
+      <c r="P61" s="113"/>
+      <c r="Q61" s="113"/>
+      <c r="R61" s="114"/>
       <c r="S61" s="78"/>
     </row>
     <row r="62" spans="1:19" s="7" customFormat="1" ht="15">
       <c r="A62" s="74"/>
-      <c r="B62" s="97"/>
-      <c r="C62" s="95"/>
+      <c r="B62" s="116"/>
+      <c r="C62" s="100"/>
       <c r="D62" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="102" t="s">
+      <c r="E62" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="101"/>
-      <c r="G62" s="101"/>
-      <c r="H62" s="99" t="s">
+      <c r="F62" s="108"/>
+      <c r="G62" s="108"/>
+      <c r="H62" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="I62" s="99"/>
-      <c r="J62" s="99"/>
+      <c r="I62" s="109"/>
+      <c r="J62" s="109"/>
       <c r="K62" s="41"/>
-      <c r="L62" s="100" t="s">
+      <c r="L62" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="M62" s="101"/>
-      <c r="N62" s="101"/>
-      <c r="O62" s="99" t="s">
+      <c r="M62" s="108"/>
+      <c r="N62" s="108"/>
+      <c r="O62" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="P62" s="99"/>
-      <c r="Q62" s="99"/>
+      <c r="P62" s="109"/>
+      <c r="Q62" s="109"/>
       <c r="R62" s="41"/>
       <c r="S62" s="79"/>
     </row>
     <row r="63" spans="1:19" s="7" customFormat="1" ht="60.75" thickBot="1">
       <c r="A63" s="74"/>
-      <c r="B63" s="98"/>
-      <c r="C63" s="96"/>
+      <c r="B63" s="117"/>
+      <c r="C63" s="101"/>
       <c r="D63" s="19" t="s">
         <v>12</v>
       </c>
@@ -4560,6 +4560,14 @@
     <row r="119" spans="1:19" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="O62:Q62"/>
+    <mergeCell ref="L62:N62"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="L61:R61"/>
+    <mergeCell ref="E61:K61"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="E2:K2"/>
@@ -4568,14 +4576,6 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="O62:Q62"/>
-    <mergeCell ref="L62:N62"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="L61:R61"/>
-    <mergeCell ref="E61:K61"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Update template (size column)
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_厚生年金保険料率一覧.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_厚生年金保険料率一覧.xlsx
@@ -1565,6 +1565,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="48" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="46" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="47" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1577,12 +1613,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="62" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1598,37 +1628,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="48" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="46" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="47" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1951,14 +1951,14 @@
   </sheetPr>
   <dimension ref="A1:S119"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="40" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="40" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="42" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="13" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1973,7 +1973,7 @@
     <col min="16" max="16" width="11.140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="1" style="1" customWidth="1"/>
     <col min="21" max="21" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1984,7 +1984,7 @@
     <col min="29" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.4" customHeight="1" thickBot="1">
+    <row r="1" spans="1:19" ht="20.25" customHeight="1" thickBot="1">
       <c r="B1" s="52" t="s">
         <v>27</v>
       </c>
@@ -1999,68 +1999,68 @@
       </c>
       <c r="S1" s="21"/>
     </row>
-    <row r="2" spans="1:19" s="7" customFormat="1" ht="15.75" thickTop="1">
-      <c r="B2" s="96" t="s">
+    <row r="2" spans="1:19" s="7" customFormat="1" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="111" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="54"/>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="105" t="s">
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="106"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="116"/>
       <c r="S2" s="55"/>
     </row>
     <row r="3" spans="1:19" s="7" customFormat="1" ht="15">
-      <c r="B3" s="97"/>
-      <c r="C3" s="100"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="96"/>
       <c r="D3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="109" t="s">
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="109"/>
-      <c r="J3" s="110"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="117"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="111" t="s">
+      <c r="L3" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="109" t="s">
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="110"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="117"/>
       <c r="R3" s="93"/>
       <c r="S3" s="55"/>
     </row>
     <row r="4" spans="1:19" s="7" customFormat="1" ht="60.75" thickBot="1">
       <c r="A4" s="74"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="101"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="19" t="s">
         <v>22</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="R59" s="66"/>
       <c r="S59" s="51"/>
     </row>
-    <row r="60" spans="1:19" ht="15.4" customHeight="1" thickTop="1" thickBot="1">
+    <row r="60" spans="1:19" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B60" s="52" t="s">
         <v>28</v>
       </c>
@@ -3289,70 +3289,70 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:19" s="7" customFormat="1" ht="15.75" thickTop="1">
+    <row r="61" spans="1:19" s="7" customFormat="1" ht="19.5" customHeight="1" thickTop="1">
       <c r="A61" s="74"/>
-      <c r="B61" s="116" t="s">
+      <c r="B61" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="100" t="s">
+      <c r="C61" s="96" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="18"/>
-      <c r="E61" s="115" t="s">
+      <c r="E61" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="F61" s="113"/>
-      <c r="G61" s="113"/>
-      <c r="H61" s="113"/>
-      <c r="I61" s="113"/>
-      <c r="J61" s="113"/>
-      <c r="K61" s="114"/>
-      <c r="L61" s="112" t="s">
+      <c r="F61" s="105"/>
+      <c r="G61" s="105"/>
+      <c r="H61" s="105"/>
+      <c r="I61" s="105"/>
+      <c r="J61" s="105"/>
+      <c r="K61" s="106"/>
+      <c r="L61" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="M61" s="113"/>
-      <c r="N61" s="113"/>
-      <c r="O61" s="113"/>
-      <c r="P61" s="113"/>
-      <c r="Q61" s="113"/>
-      <c r="R61" s="114"/>
+      <c r="M61" s="105"/>
+      <c r="N61" s="105"/>
+      <c r="O61" s="105"/>
+      <c r="P61" s="105"/>
+      <c r="Q61" s="105"/>
+      <c r="R61" s="106"/>
       <c r="S61" s="78"/>
     </row>
     <row r="62" spans="1:19" s="7" customFormat="1" ht="15">
       <c r="A62" s="74"/>
-      <c r="B62" s="116"/>
-      <c r="C62" s="100"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="96"/>
       <c r="D62" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="107" t="s">
+      <c r="E62" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="108"/>
-      <c r="G62" s="108"/>
-      <c r="H62" s="109" t="s">
+      <c r="F62" s="102"/>
+      <c r="G62" s="102"/>
+      <c r="H62" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="I62" s="109"/>
-      <c r="J62" s="109"/>
+      <c r="I62" s="100"/>
+      <c r="J62" s="100"/>
       <c r="K62" s="41"/>
-      <c r="L62" s="111" t="s">
+      <c r="L62" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="M62" s="108"/>
-      <c r="N62" s="108"/>
-      <c r="O62" s="109" t="s">
+      <c r="M62" s="102"/>
+      <c r="N62" s="102"/>
+      <c r="O62" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="P62" s="109"/>
-      <c r="Q62" s="109"/>
+      <c r="P62" s="100"/>
+      <c r="Q62" s="100"/>
       <c r="R62" s="41"/>
       <c r="S62" s="79"/>
     </row>
     <row r="63" spans="1:19" s="7" customFormat="1" ht="60.75" thickBot="1">
       <c r="A63" s="74"/>
-      <c r="B63" s="117"/>
-      <c r="C63" s="101"/>
+      <c r="B63" s="99"/>
+      <c r="C63" s="97"/>
       <c r="D63" s="19" t="s">
         <v>12</v>
       </c>
@@ -4560,6 +4560,14 @@
     <row r="119" spans="1:19" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:Q3"/>
     <mergeCell ref="C61:C63"/>
     <mergeCell ref="B61:B63"/>
     <mergeCell ref="O62:Q62"/>
@@ -4568,18 +4576,10 @@
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="L61:R61"/>
     <mergeCell ref="E61:K61"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,標準"&amp;10日通システム株式会社
 &amp;C&amp;"ＭＳ ゴシック,標準"&amp;16厚生年金保険料率一覧 &amp;R&amp;"ＭＳ ゴシック,標準"&amp;10 &amp;KFF0000 &amp;K01+000 &amp;D　&amp;T　

</xml_diff>